<commit_message>
implemented save to excel header; GroupSessionResultsReport and model
</commit_message>
<xml_diff>
--- a/Task07/EXCLFiles/AllResultsByGroup№11.xlsx
+++ b/Task07/EXCLFiles/AllResultsByGroup№11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\visual_studio\GitHub\.NET-GSTU-Autumn-2019\Task06\src\DatabaseDevelopmentConsoleApp\ConsoleApp1\bin\Debug\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\visual_studio\GitHub\.NET-GSTU-Autumn-2019\Task07\EXCLFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>Данныестудента</t>
   </si>
 </sst>
 </file>
@@ -135,9 +138,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -418,9 +424,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -711,7 +719,21 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:H9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>